<commit_message>
Excel files needs to be updated to be suited with excel importer sheets
</commit_message>
<xml_diff>
--- a/tests/stubs/2sheets2000rows.xlsx
+++ b/tests/stubs/2sheets2000rows.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad Akbari\Documents\excel-importer-enterprise\tests\stubs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14B9AA51-A2A5-43AD-AA52-1DE06275E2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B6901D-469D-42D2-8E6F-52CAB7766726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5B16EF85-512F-4730-8F43-1AC2E7ADA3CD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -374,7 +374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEB708A-3391-42A7-A98F-E1C028146850}">
   <dimension ref="A1:A2000"/>
   <sheetViews>
-    <sheetView topLeftCell="A1974" workbookViewId="0"/>
+    <sheetView topLeftCell="A1986" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -10387,8 +10387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDAA7C3-691B-44BF-A667-4CF2C73157DA}">
   <dimension ref="A1:A2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A1974" workbookViewId="0">
+      <selection activeCell="L1984" sqref="L1984"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>